<commit_message>
Added comments to manuscript.
</commit_message>
<xml_diff>
--- a/Processed Data/Classified images/FRAGSTATS_results/FRAGSTAT_Summary.xlsx
+++ b/Processed Data/Classified images/FRAGSTATS_results/FRAGSTAT_Summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boisrame\Documents\GitHub\FireWater\SEKI_Imagery_Analysis\Processed Data\Classified images\FRAGSTATS_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\SEKI_Imagery_Analysis\Processed Data\Classified images\FRAGSTATS_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -9020,16 +9020,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9499,16 +9499,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9796,12 +9796,12 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="1" max="1" width="132.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -10299,8 +10299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="AG26" sqref="AG26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>